<commit_message>
Wnioski i analiza przyspieszenia
</commit_message>
<xml_diff>
--- a/wzniki + nowe/wyniki wszystkie.xlsx
+++ b/wzniki + nowe/wyniki wszystkie.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="510" yWindow="915" windowWidth="28050" windowHeight="11670" activeTab="4"/>
+    <workbookView xWindow="510" yWindow="975" windowWidth="28050" windowHeight="11610" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="3 pętle równolegle" sheetId="1" r:id="rId1"/>
@@ -14,12 +14,11 @@
     <sheet name="Wyreksy" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="144525"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="58">
   <si>
     <t xml:space="preserve"> Source Code</t>
   </si>
@@ -187,6 +186,12 @@
   </si>
   <si>
     <t>3-sekwencyjnie</t>
+  </si>
+  <si>
+    <t>Przyspieszenie</t>
+  </si>
+  <si>
+    <t>Czas przetwarzania</t>
   </si>
 </sst>
 </file>
@@ -596,11 +601,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="56164736"/>
-        <c:axId val="56166656"/>
+        <c:axId val="163952896"/>
+        <c:axId val="164757504"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="56164736"/>
+        <c:axId val="163952896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -610,7 +615,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="56166656"/>
+        <c:crossAx val="164757504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -618,7 +623,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="56166656"/>
+        <c:axId val="164757504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -629,7 +634,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="56164736"/>
+        <c:crossAx val="163952896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -836,11 +841,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="182905472"/>
-        <c:axId val="182937472"/>
+        <c:axId val="164783616"/>
+        <c:axId val="164785152"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="182905472"/>
+        <c:axId val="164783616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -850,7 +855,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="182937472"/>
+        <c:crossAx val="164785152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -858,7 +863,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="182937472"/>
+        <c:axId val="164785152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -869,7 +874,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="182905472"/>
+        <c:crossAx val="164783616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1076,11 +1081,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="172582784"/>
-        <c:axId val="182738944"/>
+        <c:axId val="164836096"/>
+        <c:axId val="164837632"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="172582784"/>
+        <c:axId val="164836096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1090,7 +1095,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="182738944"/>
+        <c:crossAx val="164837632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1098,7 +1103,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="182738944"/>
+        <c:axId val="164837632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1109,7 +1114,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="172582784"/>
+        <c:crossAx val="164836096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1316,11 +1321,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="182964608"/>
-        <c:axId val="183066624"/>
+        <c:axId val="164864000"/>
+        <c:axId val="164865536"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="182964608"/>
+        <c:axId val="164864000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1330,7 +1335,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="183066624"/>
+        <c:crossAx val="164865536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1338,7 +1343,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="183066624"/>
+        <c:axId val="164865536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1349,7 +1354,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="182964608"/>
+        <c:crossAx val="164864000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1556,11 +1561,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="183119872"/>
-        <c:axId val="183121408"/>
+        <c:axId val="166607872"/>
+        <c:axId val="166609664"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="183119872"/>
+        <c:axId val="166607872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1570,7 +1575,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="183121408"/>
+        <c:crossAx val="166609664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1578,7 +1583,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="183121408"/>
+        <c:axId val="166609664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1589,7 +1594,457 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="183119872"/>
+        <c:crossAx val="166607872"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pl-PL"/>
+              <a:t>Czas przetwarzania</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Wyreksy!$E$87</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>3 – równolegle</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Wyreksy!$D$88:$D$90</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1400</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1600</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Wyreksy!$E$88:$E$90</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>5.335</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.2210000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.6280000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Wyreksy!$F$87</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>6 – równolegle</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Wyreksy!$D$88:$D$90</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1400</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1600</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Wyreksy!$F$88:$F$90</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.57799999999999996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.31</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.36</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Wyreksy!$G$87</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>3-sekwencyjnie</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Wyreksy!$D$88:$D$90</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1400</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1600</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Wyreksy!$G$88:$G$90</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1.395</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.6890000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.302</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="187236352"/>
+        <c:axId val="187237888"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="187236352"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="187237888"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="187237888"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="187236352"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pl-PL"/>
+              <a:t>Analiza przyspieszenia</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Wyreksy!$E$95</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>3 – równolegle</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Wyreksy!$D$96:$D$98</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1400</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1600</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Wyreksy!$E$96:$E$98</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.26148078725398316</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.27149975888120881</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.26680574872508112</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Wyreksy!$F$95</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>6 – równolegle</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Wyreksy!$F$96:$F$98</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>2.4134948096885815</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.4483870967741934</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.3944444444444448</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="171319296"/>
+        <c:axId val="171320832"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="171319296"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="171320832"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="171320832"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="171319296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1764,6 +2219,66 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>463826</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>24019</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>265043</xdr:colOff>
+      <xdr:row>102</xdr:row>
+      <xdr:rowOff>91937</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>417029</xdr:colOff>
+      <xdr:row>105</xdr:row>
+      <xdr:rowOff>140804</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>125</xdr:row>
+      <xdr:rowOff>65846</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3686,10 +4201,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B5:G74"/>
+  <dimension ref="B5:G98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AH14" sqref="AH14"/>
+    <sheetView tabSelected="1" topLeftCell="A83" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T110" sqref="T110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
@@ -4294,6 +4809,122 @@
         <v>0</v>
       </c>
     </row>
+    <row r="86" spans="4:7">
+      <c r="D86" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="87" spans="4:7">
+      <c r="D87" t="s">
+        <v>47</v>
+      </c>
+      <c r="E87" t="s">
+        <v>48</v>
+      </c>
+      <c r="F87" t="s">
+        <v>54</v>
+      </c>
+      <c r="G87" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="88" spans="4:7">
+      <c r="D88">
+        <v>1400</v>
+      </c>
+      <c r="E88">
+        <v>5.335</v>
+      </c>
+      <c r="F88">
+        <v>0.57799999999999996</v>
+      </c>
+      <c r="G88">
+        <v>1.395</v>
+      </c>
+    </row>
+    <row r="89" spans="4:7">
+      <c r="D89">
+        <v>1500</v>
+      </c>
+      <c r="E89">
+        <v>6.2210000000000001</v>
+      </c>
+      <c r="F89">
+        <v>0.31</v>
+      </c>
+      <c r="G89">
+        <v>1.6890000000000001</v>
+      </c>
+    </row>
+    <row r="90" spans="4:7">
+      <c r="D90">
+        <v>1600</v>
+      </c>
+      <c r="E90">
+        <v>8.6280000000000001</v>
+      </c>
+      <c r="F90">
+        <v>0.36</v>
+      </c>
+      <c r="G90">
+        <v>2.302</v>
+      </c>
+    </row>
+    <row r="94" spans="4:7">
+      <c r="D94" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="95" spans="4:7">
+      <c r="D95" t="s">
+        <v>47</v>
+      </c>
+      <c r="E95" t="s">
+        <v>48</v>
+      </c>
+      <c r="F95" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="96" spans="4:7">
+      <c r="D96">
+        <v>1400</v>
+      </c>
+      <c r="E96">
+        <f>G88/E88</f>
+        <v>0.26148078725398316</v>
+      </c>
+      <c r="F96">
+        <f>G88/F88</f>
+        <v>2.4134948096885815</v>
+      </c>
+    </row>
+    <row r="97" spans="4:6">
+      <c r="D97">
+        <v>1500</v>
+      </c>
+      <c r="E97">
+        <f t="shared" ref="E97:E98" si="0">G89/E89</f>
+        <v>0.27149975888120881</v>
+      </c>
+      <c r="F97">
+        <f t="shared" ref="F97:F98" si="1">G89/F89</f>
+        <v>5.4483870967741934</v>
+      </c>
+    </row>
+    <row r="98" spans="4:6">
+      <c r="D98">
+        <v>1600</v>
+      </c>
+      <c r="E98">
+        <f t="shared" si="0"/>
+        <v>0.26680574872508112</v>
+      </c>
+      <c r="F98">
+        <f t="shared" si="1"/>
+        <v>6.3944444444444448</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0" right="0" top="0.39370078740157477" bottom="0.39370078740157477" header="0" footer="0"/>
   <headerFooter>

</xml_diff>